<commit_message>
sum in inventory tab and delivery price in ordering tab and other modifications
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="محصولات" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="126">
   <si>
     <t>SKU</t>
   </si>
@@ -141,9 +141,6 @@
     <t>هدست بلوتوثی مدل S530 با کیفیت مناسب</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>135</t>
   </si>
   <si>
@@ -195,7 +192,7 @@
     <t>66</t>
   </si>
   <si>
-    <t>هدست بلوتوث طرح جبرا با قیمت و کیفیت مناسب نسبت به هدست های مشابه</t>
+    <t>هدست بلوتوث طرح جبرا با قیمت و کیفیت مناسب نسبت به هدست های مشابه (از تاریخ 11/04/1398 با تخفیف 19 هزار تومانی برای مشتریان گرامی ارسال خواهد شد و قیمت از 69 هزار تومان به 50 هزار تومان کاهش خواهد یافت)</t>
   </si>
   <si>
     <t>EB-716092</t>
@@ -249,6 +246,9 @@
     <t>پنکه رومیزی با باددهی مناسب جهت استفاده در میز کار و تحریر</t>
   </si>
   <si>
+    <t>170</t>
+  </si>
+  <si>
     <t>EB-718127</t>
   </si>
   <si>
@@ -318,6 +318,9 @@
     <t>EB-724892</t>
   </si>
   <si>
+    <t>هندزفری بلوتوث اسپورت Sport</t>
+  </si>
+  <si>
     <t>13980408</t>
   </si>
   <si>
@@ -327,13 +330,73 @@
     <t>EB-724894</t>
   </si>
   <si>
-    <t>پد عرقگیر</t>
+    <t>پد ضد عرق نانو</t>
   </si>
   <si>
     <t>پد عرقگیر مناسب فصل تابستان برای جلوگیری از انتقال تعریق بدن به لباس</t>
   </si>
   <si>
-    <t>هندزفری بلوتوث اسپورت</t>
+    <t>EB-725974</t>
+  </si>
+  <si>
+    <t>هدست بلوتوث دورگردنی ال جی</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>13980410</t>
+  </si>
+  <si>
+    <t>هدست بلوتوث دورگردنی ال جی با کیفیت مناسب</t>
+  </si>
+  <si>
+    <t>EB-725975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هدست بلوتوث دورگردنی سامسونگ </t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>هدست بلوتوث دورگردنی سامسونگ با کیفیت مناسب</t>
+  </si>
+  <si>
+    <t>EB-728219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تگ ضد سرقت </t>
+  </si>
+  <si>
+    <t>13980416</t>
+  </si>
+  <si>
+    <t>تگ ضد سرقت با کیفیت مناسب و خوب&amp;nbsp;</t>
+  </si>
+  <si>
+    <t>EB-731817</t>
+  </si>
+  <si>
+    <t>تقویت کننده  ۱۵۰ گرمی با کوپلینگ</t>
+  </si>
+  <si>
+    <t>1398/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تقویت کننده  ۱۵۰ گرمی با کوپلینگ با کیفیت مناسب </t>
+  </si>
+  <si>
+    <t>EB-731819</t>
+  </si>
+  <si>
+    <t>شارژ گاز فریز ۲۵۰ گرم R134a با کوپلینگ</t>
+  </si>
+  <si>
+    <t>270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شارژ گاز فریز ۲۵۰ گرم R134a با کوپلینگ با کیفیت مناسب </t>
   </si>
 </sst>
 </file>
@@ -400,8 +463,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H23" totalsRowShown="0">
-  <autoFilter ref="A1:H23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H28" totalsRowShown="0">
+  <autoFilter ref="A1:H28"/>
   <tableColumns count="8">
     <tableColumn id="1" name="SKU"/>
     <tableColumn id="2" name="نام محصول"/>
@@ -701,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -714,9 +777,9 @@
     <col min="3" max="3" width="10.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="7.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="159.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="169.33203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
@@ -764,7 +827,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="1">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>12</v>
@@ -790,7 +853,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -816,7 +879,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
@@ -842,7 +905,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="1">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
@@ -868,7 +931,7 @@
         <v>28</v>
       </c>
       <c r="F6" s="1">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
@@ -894,7 +957,7 @@
         <v>33</v>
       </c>
       <c r="F7" s="1">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>29</v>
@@ -920,7 +983,7 @@
         <v>37</v>
       </c>
       <c r="F8" s="1">
-        <v>323</v>
+        <v>189</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>38</v>
@@ -931,10 +994,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C9" s="1">
         <v>1290000</v>
@@ -943,24 +1006,24 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="1">
-        <v>31</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C10" s="1">
         <v>590000</v>
@@ -969,24 +1032,24 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="1">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F10" s="1">
-        <v>32</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C11" s="1">
         <v>1050000</v>
@@ -995,50 +1058,50 @@
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="1">
+        <v>37</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F11" s="1">
-        <v>36</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1">
+        <v>500000</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="1">
-        <v>690000</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1">
+        <v>76</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F12" s="1">
-        <v>37</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="C13" s="1">
         <v>990000</v>
@@ -1047,24 +1110,24 @@
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="1">
+        <v>49</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F13" s="1">
-        <v>5</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="C14" s="1">
         <v>890000</v>
@@ -1073,24 +1136,24 @@
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C15" s="1">
         <v>1700000</v>
@@ -1099,24 +1162,24 @@
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15" s="1">
         <v>40</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C16" s="1">
         <v>690000</v>
@@ -1125,16 +1188,16 @@
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="1">
+        <v>40</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="1">
-        <v>41</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1154,7 +1217,7 @@
         <v>78</v>
       </c>
       <c r="F17" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>79</v>
@@ -1180,7 +1243,7 @@
         <v>33</v>
       </c>
       <c r="F18" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>83</v>
@@ -1229,10 +1292,10 @@
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="1">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>92</v>
@@ -1258,7 +1321,7 @@
         <v>33</v>
       </c>
       <c r="F21" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>96</v>
@@ -1272,51 +1335,181 @@
         <v>98</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C22" s="1">
-        <v>590000</v>
+        <v>690000</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="F22" s="1">
+        <v>46</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C23" s="1">
-        <v>500000</v>
+        <v>350000</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="F23" s="1">
+        <v>41</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1450000</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="1">
+        <v>17</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1250000</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="1">
+        <v>15</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="1">
+        <v>850000</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="1">
+        <v>710000</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1400000</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>